<commit_message>
added small data set and minor fixes
</commit_message>
<xml_diff>
--- a/data/eltypes.xlsx
+++ b/data/eltypes.xlsx
@@ -27,15 +27,9 @@
     <t>EXPOSURE</t>
   </si>
   <si>
-    <t>LOSS20</t>
-  </si>
-  <si>
     <t>PREMIUM66</t>
   </si>
   <si>
-    <t>SCHAEDEN_ANZAHL</t>
-  </si>
-  <si>
     <t>MALLORCA_POLICE</t>
   </si>
   <si>
@@ -129,36 +123,6 @@
     <t>FUEHRERSCHEIN_ERWORBEN_AM</t>
   </si>
   <si>
-    <t>schaeden0_typeKH</t>
-  </si>
-  <si>
-    <t>schaeden0_typetk</t>
-  </si>
-  <si>
-    <t>schaeden0_month</t>
-  </si>
-  <si>
-    <t>schaeden0_year</t>
-  </si>
-  <si>
-    <t>schaeden1_typetk</t>
-  </si>
-  <si>
-    <t>schaeden1_month</t>
-  </si>
-  <si>
-    <t>schaeden1_year</t>
-  </si>
-  <si>
-    <t>schaeden2_typevk</t>
-  </si>
-  <si>
-    <t>schaeden2_month</t>
-  </si>
-  <si>
-    <t>schaeden2_year</t>
-  </si>
-  <si>
     <t>scrapedate</t>
   </si>
   <si>
@@ -364,6 +328,42 @@
   </si>
   <si>
     <t>Eltypes</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN_ANZAHL</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN0_typeKH</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN0_typetk</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN0_month</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN0_year</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN1_typetk</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN1_month</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN1_year</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN2_typevk</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN2_month</t>
+  </si>
+  <si>
+    <t>VORSCHAEDEN2_year</t>
+  </si>
+  <si>
+    <t>LOSS20HALF</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1171,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK6"/>
+  <dimension ref="A1:CK8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
@@ -1179,16 +1179,16 @@
   <sheetData>
     <row r="1" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:89" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
-        <f>+IF(ISNUMBER(A6),IF(INT(A6)=A6,"Int64","Float64"),"String")</f>
+        <f>+IF(ISNUMBER(A8),IF(INT(A8)=A8,"Int64","Float64"),"String")</f>
         <v>Int64</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:BM2" si="0">+IF(ISNUMBER(B6),IF(INT(B6)=B6,"Int64","Float64"),"String")</f>
+        <f t="shared" ref="B2:BM2" si="0">+IF(ISNUMBER(B8),IF(INT(B8)=B8,"Int64","Float64"),"String")</f>
         <v>Float64</v>
       </c>
       <c r="C2" t="str">
@@ -1444,7 +1444,7 @@
         <v>Int64</v>
       </c>
       <c r="BN2" t="str">
-        <f t="shared" ref="BN2:CK2" si="1">+IF(ISNUMBER(BN6),IF(INT(BN6)=BN6,"Int64","Float64"),"String")</f>
+        <f t="shared" ref="BN2:CK2" si="1">+IF(ISNUMBER(BN8),IF(INT(BN8)=BN8,"Int64","Float64"),"String")</f>
         <v>Int64</v>
       </c>
       <c r="BO2" t="str">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="BZ2" t="str">
         <f t="shared" si="1"/>
-        <v>Int64</v>
+        <v>Float64</v>
       </c>
       <c r="CA2" t="str">
         <f t="shared" si="1"/>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="BZ3" t="str">
         <f t="shared" si="3"/>
-        <v>Int64,</v>
+        <v>Float64,</v>
       </c>
       <c r="CA3" t="str">
         <f t="shared" si="3"/>
@@ -1898,541 +1898,1253 @@
         <v>Int64,</v>
       </c>
     </row>
+    <row r="4" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="B4" t="str">
+        <f>+""""&amp;B7&amp;""""&amp;","</f>
+        <v>"EXPOSURE",</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:BN4" si="4">+""""&amp;C7&amp;""""&amp;","</f>
+        <v>"LOSS20HALF",</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="4"/>
+        <v>"PREMIUM66",</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN_ANZAHL",</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="4"/>
+        <v>"MALLORCA_POLICE",</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="4"/>
+        <v>"SCHUTZBRIEF_INKL",</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="4"/>
+        <v>"FREIE_WERKSTATTWAHL",</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="4"/>
+        <v>"AUTOMOBILCLUB_MITGLIED_SEIT",</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="4"/>
+        <v>"BAHNCARD",</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>"ZAHLUNGSWEISE",</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="4"/>
+        <v>"JAHRESKARTE_OEPNV",</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>"MOTORRAD_BESITZER",</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="4"/>
+        <v>"AUTOMOBILCLUB",</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="4"/>
+        <v>"SFKLASSE_VOLLKASKO",</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="4"/>
+        <v>"SFKLASSE_HAFTPFLICHT",</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="4"/>
+        <v>"STELLPLATZ_ABSCHLIESSBAR",</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="4"/>
+        <v>"NAECHTLICHER_STELLPLATZ",</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" si="4"/>
+        <v>"NUTZUNGSWEISE",</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="4"/>
+        <v>"JAEHRLICHE_FAHRLEISTUNG",</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="4"/>
+        <v>"TSN",</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="4"/>
+        <v>"ERSTZULASSUNG",</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="4"/>
+        <v>"HSN",</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="4"/>
+        <v>"FINANZIERUNGSART",</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="4"/>
+        <v>"ZULASSUNG_AUF_VERSICHERUNGSNEHM",</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" si="4"/>
+        <v>"STADT",</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="4"/>
+        <v>"KENNZEICHEN",</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="4"/>
+        <v>"PLZ_DES_HALTER",</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="4"/>
+        <v>"SELBSTGENUTZTES_WOHNEIGENTUM",</v>
+      </c>
+      <c r="AD4" t="str">
+        <f t="shared" si="4"/>
+        <v>"ART_DES_WOHNEIGENTUM",</v>
+      </c>
+      <c r="AE4" t="str">
+        <f t="shared" si="4"/>
+        <v>"GEBURTSDATUM",</v>
+      </c>
+      <c r="AF4" t="str">
+        <f t="shared" si="4"/>
+        <v>"FAMILIENSTAND",</v>
+      </c>
+      <c r="AG4" t="str">
+        <f t="shared" si="4"/>
+        <v>"NATIONALITAET",</v>
+      </c>
+      <c r="AH4" t="str">
+        <f t="shared" si="4"/>
+        <v>"PLZ_WOHNORT",</v>
+      </c>
+      <c r="AI4" t="str">
+        <f t="shared" si="4"/>
+        <v>"GESCHLECHT",</v>
+      </c>
+      <c r="AJ4" t="str">
+        <f t="shared" si="4"/>
+        <v>"FUEHRERSCHEIN_ERWORBEN_AM",</v>
+      </c>
+      <c r="AK4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN0_typeKH",</v>
+      </c>
+      <c r="AL4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN0_typetk",</v>
+      </c>
+      <c r="AM4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN0_month",</v>
+      </c>
+      <c r="AN4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN0_year",</v>
+      </c>
+      <c r="AO4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN1_typetk",</v>
+      </c>
+      <c r="AP4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN1_month",</v>
+      </c>
+      <c r="AQ4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN1_year",</v>
+      </c>
+      <c r="AR4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN2_typevk",</v>
+      </c>
+      <c r="AS4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN2_month",</v>
+      </c>
+      <c r="AT4" t="str">
+        <f t="shared" si="4"/>
+        <v>"VORSCHAEDEN2_year",</v>
+      </c>
+      <c r="AU4" t="str">
+        <f t="shared" si="4"/>
+        <v>"scrapedate",</v>
+      </c>
+      <c r="AV4" t="str">
+        <f t="shared" si="4"/>
+        <v>"adacid",</v>
+      </c>
+      <c r="AW4" t="str">
+        <f t="shared" si="4"/>
+        <v>"name",</v>
+      </c>
+      <c r="AX4" t="str">
+        <f t="shared" si="4"/>
+        <v>"marke",</v>
+      </c>
+      <c r="AY4" t="str">
+        <f t="shared" si="4"/>
+        <v>"modell",</v>
+      </c>
+      <c r="AZ4" t="str">
+        <f t="shared" si="4"/>
+        <v>"preis",</v>
+      </c>
+      <c r="BA4" t="str">
+        <f t="shared" si="4"/>
+        <v>"getriebeart",</v>
+      </c>
+      <c r="BB4" t="str">
+        <f t="shared" si="4"/>
+        <v>"antriebsart",</v>
+      </c>
+      <c r="BC4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Fahrzeugklasse",</v>
+      </c>
+      <c r="BD4" t="str">
+        <f t="shared" si="4"/>
+        <v>"co2klasse",</v>
+      </c>
+      <c r="BE4" t="str">
+        <f t="shared" si="4"/>
+        <v>"kw",</v>
+      </c>
+      <c r="BF4" t="str">
+        <f t="shared" si="4"/>
+        <v>"ps",</v>
+      </c>
+      <c r="BG4" t="str">
+        <f t="shared" si="4"/>
+        <v>"tueranzahl",</v>
+      </c>
+      <c r="BH4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Motorart",</v>
+      </c>
+      <c r="BI4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Kraftstoffart",</v>
+      </c>
+      <c r="BJ4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Motorbauart",</v>
+      </c>
+      <c r="BK4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Schadstoffklasse",</v>
+      </c>
+      <c r="BL4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Karosserie",</v>
+      </c>
+      <c r="BM4" t="str">
+        <f t="shared" si="4"/>
+        <v>"Sitzanzahl",</v>
+      </c>
+      <c r="BN4" t="str">
+        <f t="shared" si="4"/>
+        <v>"typklasseh_num",</v>
+      </c>
+      <c r="BO4" t="str">
+        <f t="shared" ref="BO4:CK4" si="5">+""""&amp;BO7&amp;""""&amp;","</f>
+        <v>"typklassetk_num",</v>
+      </c>
+      <c r="BP4" t="str">
+        <f t="shared" si="5"/>
+        <v>"typklassevk_num",</v>
+      </c>
+      <c r="BQ4" t="str">
+        <f t="shared" si="5"/>
+        <v>"hubraum2",</v>
+      </c>
+      <c r="BR4" t="str">
+        <f t="shared" si="5"/>
+        <v>"drehmoment2",</v>
+      </c>
+      <c r="BS4" t="str">
+        <f t="shared" si="5"/>
+        <v>"breite2",</v>
+      </c>
+      <c r="BT4" t="str">
+        <f t="shared" si="5"/>
+        <v>"radstand2",</v>
+      </c>
+      <c r="BU4" t="str">
+        <f t="shared" si="5"/>
+        <v>"laenge2",</v>
+      </c>
+      <c r="BV4" t="str">
+        <f t="shared" si="5"/>
+        <v>"hoehe2",</v>
+      </c>
+      <c r="BW4" t="str">
+        <f t="shared" si="5"/>
+        <v>"leergewicht2",</v>
+      </c>
+      <c r="BX4" t="str">
+        <f t="shared" si="5"/>
+        <v>"gesamtgewicht2",</v>
+      </c>
+      <c r="BY4" t="str">
+        <f t="shared" si="5"/>
+        <v>"zuladung2",</v>
+      </c>
+      <c r="BZ4" t="str">
+        <f t="shared" si="5"/>
+        <v>"kofferraumvolumen_num",</v>
+      </c>
+      <c r="CA4" t="str">
+        <f t="shared" si="5"/>
+        <v>"hoechstgeschwindigkeit2",</v>
+      </c>
+      <c r="CB4" t="str">
+        <f t="shared" si="5"/>
+        <v>"verbrauchgesamt2",</v>
+      </c>
+      <c r="CC4" t="str">
+        <f t="shared" si="5"/>
+        <v>"verbrauchausserorts2",</v>
+      </c>
+      <c r="CD4" t="str">
+        <f t="shared" si="5"/>
+        <v>"verbrauchinnerorts2",</v>
+      </c>
+      <c r="CE4" t="str">
+        <f t="shared" si="5"/>
+        <v>"beschleunigung2",</v>
+      </c>
+      <c r="CF4" t="str">
+        <f t="shared" si="5"/>
+        <v>"tank2",</v>
+      </c>
+      <c r="CG4" t="str">
+        <f t="shared" si="5"/>
+        <v>"kfzsteuer2",</v>
+      </c>
+      <c r="CH4" t="str">
+        <f t="shared" si="5"/>
+        <v>"anzahlgaenge2",</v>
+      </c>
+      <c r="CI4" t="str">
+        <f t="shared" si="5"/>
+        <v>"anzahlzylinder2",</v>
+      </c>
+      <c r="CJ4" t="str">
+        <f t="shared" si="5"/>
+        <v>"co2_wert",</v>
+      </c>
+      <c r="CK4" t="str">
+        <f t="shared" si="5"/>
+        <v>"modellstart_y",</v>
+      </c>
+    </row>
     <row r="5" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5">
+        <f>+COLUMN()</f>
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:BM5" si="6">+COLUMN()</f>
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="6"/>
+        <v>24</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="6"/>
+        <v>27</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="6"/>
+        <v>29</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="6"/>
+        <v>33</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="6"/>
+        <v>34</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="AJ5">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="6"/>
+        <v>39</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="6"/>
+        <v>41</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="6"/>
+        <v>42</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="6"/>
+        <v>43</v>
+      </c>
+      <c r="AR5">
+        <f t="shared" si="6"/>
+        <v>44</v>
+      </c>
+      <c r="AS5">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="AT5">
+        <f t="shared" si="6"/>
+        <v>46</v>
+      </c>
+      <c r="AU5">
+        <f t="shared" si="6"/>
+        <v>47</v>
+      </c>
+      <c r="AV5">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="AW5">
+        <f t="shared" si="6"/>
+        <v>49</v>
+      </c>
+      <c r="AX5">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
+      <c r="AY5">
+        <f t="shared" si="6"/>
+        <v>51</v>
+      </c>
+      <c r="AZ5">
+        <f t="shared" si="6"/>
+        <v>52</v>
+      </c>
+      <c r="BA5">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="BB5">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="BC5">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+      <c r="BD5">
+        <f t="shared" si="6"/>
+        <v>56</v>
+      </c>
+      <c r="BE5">
+        <f t="shared" si="6"/>
+        <v>57</v>
+      </c>
+      <c r="BF5">
+        <f t="shared" si="6"/>
+        <v>58</v>
+      </c>
+      <c r="BG5">
+        <f t="shared" si="6"/>
+        <v>59</v>
+      </c>
+      <c r="BH5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="BI5">
+        <f t="shared" si="6"/>
+        <v>61</v>
+      </c>
+      <c r="BJ5">
+        <f t="shared" si="6"/>
+        <v>62</v>
+      </c>
+      <c r="BK5">
+        <f t="shared" si="6"/>
+        <v>63</v>
+      </c>
+      <c r="BL5">
+        <f t="shared" si="6"/>
+        <v>64</v>
+      </c>
+      <c r="BM5">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="BN5">
+        <f t="shared" ref="BN5:CK5" si="7">+COLUMN()</f>
+        <v>66</v>
+      </c>
+      <c r="BO5">
+        <f t="shared" si="7"/>
+        <v>67</v>
+      </c>
+      <c r="BP5">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="BQ5">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="BR5">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="BS5">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="BT5">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="BU5">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="BV5">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+      <c r="BW5">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="BX5">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="BY5">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="BZ5">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="CA5">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+      <c r="CB5">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="CC5">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="CD5">
+        <f t="shared" si="7"/>
+        <v>82</v>
+      </c>
+      <c r="CE5">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+      <c r="CF5">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+      <c r="CG5">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="CH5">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+      <c r="CI5">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="CJ5">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="CK5">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H7" t="s">
         <v>5</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I7" t="s">
         <v>6</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J7" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K7" t="s">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L7" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M7" t="s">
         <v>10</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N7" t="s">
         <v>11</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P7" t="s">
         <v>13</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q7" t="s">
         <v>14</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R7" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S7" t="s">
         <v>16</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T7" t="s">
         <v>17</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U7" t="s">
         <v>18</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V7" t="s">
         <v>19</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W7" t="s">
         <v>20</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X7" t="s">
         <v>21</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y7" t="s">
         <v>22</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z7" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA7" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB7" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC7" t="s">
         <v>26</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD7" t="s">
         <v>27</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AE7" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AF7" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG7" t="s">
         <v>30</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AH7" t="s">
         <v>31</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AI7" t="s">
         <v>32</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AJ7" t="s">
         <v>33</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AK7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>106</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>109</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU7" t="s">
         <v>34</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AV7" t="s">
         <v>35</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AW7" t="s">
         <v>36</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AX7" t="s">
         <v>37</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AY7" t="s">
         <v>38</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AZ7" t="s">
         <v>39</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="BA7" t="s">
         <v>40</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="BB7" t="s">
         <v>41</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="BC7" t="s">
         <v>42</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="BD7" t="s">
         <v>43</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="BE7" t="s">
         <v>44</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="BF7" t="s">
         <v>45</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="BG7" t="s">
         <v>46</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="BH7" t="s">
         <v>47</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="BI7" t="s">
         <v>48</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="BJ7" t="s">
         <v>49</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="BK7" t="s">
         <v>50</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BL7" t="s">
         <v>51</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BM7" t="s">
         <v>52</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BN7" t="s">
         <v>53</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BO7" t="s">
         <v>54</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BP7" t="s">
         <v>55</v>
       </c>
-      <c r="BE5" t="s">
+      <c r="BQ7" t="s">
         <v>56</v>
       </c>
-      <c r="BF5" t="s">
+      <c r="BR7" t="s">
         <v>57</v>
       </c>
-      <c r="BG5" t="s">
+      <c r="BS7" t="s">
         <v>58</v>
       </c>
-      <c r="BH5" t="s">
+      <c r="BT7" t="s">
         <v>59</v>
       </c>
-      <c r="BI5" t="s">
+      <c r="BU7" t="s">
         <v>60</v>
       </c>
-      <c r="BJ5" t="s">
+      <c r="BV7" t="s">
         <v>61</v>
       </c>
-      <c r="BK5" t="s">
+      <c r="BW7" t="s">
         <v>62</v>
       </c>
-      <c r="BL5" t="s">
+      <c r="BX7" t="s">
         <v>63</v>
       </c>
-      <c r="BM5" t="s">
+      <c r="BY7" t="s">
         <v>64</v>
       </c>
-      <c r="BN5" t="s">
+      <c r="BZ7" t="s">
         <v>65</v>
       </c>
-      <c r="BO5" t="s">
+      <c r="CA7" t="s">
         <v>66</v>
       </c>
-      <c r="BP5" t="s">
+      <c r="CB7" t="s">
         <v>67</v>
       </c>
-      <c r="BQ5" t="s">
+      <c r="CC7" t="s">
         <v>68</v>
       </c>
-      <c r="BR5" t="s">
+      <c r="CD7" t="s">
         <v>69</v>
       </c>
-      <c r="BS5" t="s">
+      <c r="CE7" t="s">
         <v>70</v>
       </c>
-      <c r="BT5" t="s">
+      <c r="CF7" t="s">
         <v>71</v>
       </c>
-      <c r="BU5" t="s">
+      <c r="CG7" t="s">
         <v>72</v>
       </c>
-      <c r="BV5" t="s">
+      <c r="CH7" t="s">
         <v>73</v>
       </c>
-      <c r="BW5" t="s">
+      <c r="CI7" t="s">
         <v>74</v>
       </c>
-      <c r="BX5" t="s">
+      <c r="CJ7" t="s">
         <v>75</v>
       </c>
-      <c r="BY5" t="s">
+      <c r="CK7" t="s">
         <v>76</v>
       </c>
-      <c r="BZ5" t="s">
+    </row>
+    <row r="8" spans="1:89" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>583781</v>
+      </c>
+      <c r="B8">
+        <v>2.3022169039999998</v>
+      </c>
+      <c r="C8">
+        <v>3.1</v>
+      </c>
+      <c r="D8">
+        <v>1851.54</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>19980217</v>
+      </c>
+      <c r="J8" t="s">
         <v>77</v>
       </c>
-      <c r="CA5" t="s">
+      <c r="K8" t="s">
         <v>78</v>
       </c>
-      <c r="CB5" t="s">
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
         <v>79</v>
       </c>
-      <c r="CC5" t="s">
+      <c r="O8" t="s">
         <v>80</v>
       </c>
-      <c r="CD5" t="s">
+      <c r="P8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
         <v>81</v>
       </c>
-      <c r="CE5" t="s">
+      <c r="S8" t="s">
         <v>82</v>
       </c>
-      <c r="CF5" t="s">
+      <c r="T8">
+        <v>20</v>
+      </c>
+      <c r="U8">
+        <v>155</v>
+      </c>
+      <c r="V8">
+        <v>19941215</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8" t="s">
         <v>83</v>
       </c>
-      <c r="CG5" t="s">
+      <c r="Y8">
+        <v>20040927</v>
+      </c>
+      <c r="Z8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
         <v>84</v>
       </c>
-      <c r="CH5" t="s">
+      <c r="AB8">
+        <v>38700</v>
+      </c>
+      <c r="AC8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD8" t="s">
         <v>85</v>
       </c>
-      <c r="CI5" t="s">
+      <c r="AE8">
+        <v>19800325</v>
+      </c>
+      <c r="AF8" t="s">
         <v>86</v>
       </c>
-      <c r="CJ5" t="s">
+      <c r="AG8" t="s">
         <v>87</v>
       </c>
-      <c r="CK5" t="s">
+      <c r="AH8">
+        <v>38700</v>
+      </c>
+      <c r="AI8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:89" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>583781</v>
-      </c>
-      <c r="B6">
-        <v>2.3022169039999998</v>
-      </c>
-      <c r="C6">
-        <v>3.1</v>
-      </c>
-      <c r="D6">
-        <v>1851.54</v>
-      </c>
-      <c r="E6">
+      <c r="AJ8">
+        <v>19980210</v>
+      </c>
+      <c r="AK8" t="b">
         <v>1</v>
       </c>
-      <c r="F6" t="b">
+      <c r="AL8" t="b">
         <v>0</v>
       </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
+      <c r="AM8">
+        <v>9</v>
+      </c>
+      <c r="AN8">
+        <v>2012</v>
+      </c>
+      <c r="AO8" t="b">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>19980217</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8" t="s">
         <v>89</v>
       </c>
-      <c r="K6" t="s">
+      <c r="AV8">
+        <v>996201</v>
+      </c>
+      <c r="AW8" t="s">
         <v>90</v>
       </c>
-      <c r="L6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="AX8" t="s">
         <v>91</v>
       </c>
-      <c r="O6" t="s">
+      <c r="AY8" t="s">
         <v>92</v>
       </c>
-      <c r="P6" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="AZ8">
+        <v>72000</v>
+      </c>
+      <c r="BA8" t="s">
         <v>93</v>
       </c>
-      <c r="S6" t="s">
+      <c r="BB8" t="s">
         <v>94</v>
       </c>
-      <c r="T6">
-        <v>20</v>
-      </c>
-      <c r="U6">
-        <v>155</v>
-      </c>
-      <c r="V6">
-        <v>19941215</v>
-      </c>
-      <c r="W6">
-        <v>5</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="BC8" t="s">
         <v>95</v>
       </c>
-      <c r="Y6">
-        <v>20040927</v>
-      </c>
-      <c r="Z6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="BD8" t="s">
         <v>96</v>
       </c>
-      <c r="AB6">
-        <v>38700</v>
-      </c>
-      <c r="AC6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="s">
+      <c r="BE8">
+        <v>245</v>
+      </c>
+      <c r="BF8">
+        <v>333</v>
+      </c>
+      <c r="BG8">
+        <v>2</v>
+      </c>
+      <c r="BH8" t="s">
         <v>97</v>
       </c>
-      <c r="AE6">
-        <v>19800325</v>
-      </c>
-      <c r="AF6" t="s">
+      <c r="BI8" t="s">
         <v>98</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="BJ8" t="s">
         <v>99</v>
       </c>
-      <c r="AH6">
-        <v>38700</v>
-      </c>
-      <c r="AI6" t="s">
+      <c r="BK8" t="s">
         <v>100</v>
       </c>
-      <c r="AJ6">
-        <v>19980210</v>
-      </c>
-      <c r="AK6" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>9</v>
-      </c>
-      <c r="AN6">
-        <v>2012</v>
-      </c>
-      <c r="AO6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6" t="s">
+      <c r="BL8" t="s">
         <v>101</v>
       </c>
-      <c r="AV6">
-        <v>996201</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AZ6">
-        <v>72000</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>105</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>106</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>107</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>108</v>
-      </c>
-      <c r="BE6">
-        <v>245</v>
-      </c>
-      <c r="BF6">
-        <v>333</v>
-      </c>
-      <c r="BG6">
-        <v>2</v>
-      </c>
-      <c r="BH6" t="s">
-        <v>109</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BJ6" t="s">
-        <v>111</v>
-      </c>
-      <c r="BK6" t="s">
-        <v>112</v>
-      </c>
-      <c r="BL6" t="s">
-        <v>113</v>
-      </c>
-      <c r="BM6">
+      <c r="BM8">
         <v>4</v>
       </c>
-      <c r="BN6">
+      <c r="BN8">
         <v>21</v>
       </c>
-      <c r="BO6">
+      <c r="BO8">
         <v>28</v>
       </c>
-      <c r="BP6">
+      <c r="BP8">
         <v>30</v>
       </c>
-      <c r="BQ6">
+      <c r="BQ8">
         <v>4398</v>
       </c>
-      <c r="BR6">
+      <c r="BR8">
         <v>450</v>
       </c>
-      <c r="BS6">
+      <c r="BS8">
         <v>1855</v>
       </c>
-      <c r="BT6">
+      <c r="BT8">
         <v>2780</v>
       </c>
-      <c r="BU6">
+      <c r="BU8">
         <v>4820</v>
       </c>
-      <c r="BV6">
+      <c r="BV8">
         <v>1373</v>
       </c>
-      <c r="BW6">
+      <c r="BW8">
         <v>1690</v>
       </c>
-      <c r="BX6">
+      <c r="BX8">
         <v>2065</v>
       </c>
-      <c r="BY6">
+      <c r="BY8">
         <v>375</v>
       </c>
-      <c r="BZ6">
-        <v>45</v>
-      </c>
-      <c r="CA6">
+      <c r="BZ8">
+        <v>45.1</v>
+      </c>
+      <c r="CA8">
         <v>250</v>
       </c>
-      <c r="CB6">
+      <c r="CB8">
         <v>11.7</v>
       </c>
-      <c r="CC6">
+      <c r="CC8">
         <v>8.6</v>
       </c>
-      <c r="CD6">
+      <c r="CD8">
         <v>17.2</v>
       </c>
-      <c r="CE6">
+      <c r="CE8">
         <v>5.6</v>
       </c>
-      <c r="CF6">
+      <c r="CF8">
         <v>70</v>
       </c>
-      <c r="CG6">
+      <c r="CG8">
         <v>297</v>
       </c>
-      <c r="CH6">
+      <c r="CH8">
         <v>6</v>
       </c>
-      <c r="CI6">
+      <c r="CI8">
         <v>8</v>
       </c>
-      <c r="CJ6">
+      <c r="CJ8">
         <v>283</v>
       </c>
-      <c r="CK6">
+      <c r="CK8">
         <v>2003</v>
       </c>
     </row>

</xml_diff>